<commit_message>
Displays core + changed desired GUI
</commit_message>
<xml_diff>
--- a/desired GUI.xlsx
+++ b/desired GUI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_adulting\0_1_internships\UMD Radiation Facilities\status board\status board github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53858505-3562-4CB1-AD75-2A189D1E9B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217FCD47-AFEE-4657-93BC-7B07F58644EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4605" windowWidth="20730" windowHeight="11310" xr2:uid="{3CE19E7A-16D2-405D-A788-F282136CDB1C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3CE19E7A-16D2-405D-A788-F282136CDB1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="67">
   <si>
     <t>Thermal column</t>
   </si>
@@ -90,45 +90,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>s3</t>
-  </si>
-  <si>
-    <t>s4</t>
-  </si>
-  <si>
-    <t>s5</t>
-  </si>
-  <si>
-    <t>s6</t>
-  </si>
-  <si>
-    <t>s7</t>
-  </si>
-  <si>
-    <t>s8</t>
-  </si>
-  <si>
-    <t>s9</t>
-  </si>
-  <si>
-    <t>s10</t>
-  </si>
-  <si>
-    <t>s11</t>
-  </si>
-  <si>
-    <t>s12</t>
-  </si>
-  <si>
-    <t>s13</t>
-  </si>
-  <si>
     <t>Move Fuel</t>
   </si>
   <si>
@@ -153,9 +114,6 @@
     <t>…</t>
   </si>
   <si>
-    <t>1278x9313</t>
-  </si>
-  <si>
     <t>(x26)</t>
   </si>
   <si>
@@ -207,9 +165,6 @@
     <t>((1))</t>
   </si>
   <si>
-    <t>cellsize=49</t>
-  </si>
-  <si>
     <t>((F))</t>
   </si>
   <si>
@@ -223,6 +178,60 @@
   </si>
   <si>
     <t>((B))</t>
+  </si>
+  <si>
+    <t>Storage 1</t>
+  </si>
+  <si>
+    <t>Storage 2</t>
+  </si>
+  <si>
+    <t>Storage 3</t>
+  </si>
+  <si>
+    <t>Storage 4</t>
+  </si>
+  <si>
+    <t>Storage 5</t>
+  </si>
+  <si>
+    <t>Storage 6</t>
+  </si>
+  <si>
+    <t>Storage 7</t>
+  </si>
+  <si>
+    <t>Storage 8</t>
+  </si>
+  <si>
+    <t>Storage 9</t>
+  </si>
+  <si>
+    <t>Storage 10</t>
+  </si>
+  <si>
+    <t>Storage 11</t>
+  </si>
+  <si>
+    <t>Storage 12</t>
+  </si>
+  <si>
+    <t>Storage 13</t>
+  </si>
+  <si>
+    <t>NOPE</t>
+  </si>
+  <si>
+    <t>(x30)</t>
+  </si>
+  <si>
+    <t>cellsize=k px</t>
+  </si>
+  <si>
+    <t>k px</t>
+  </si>
+  <si>
+    <t>1278x931 on my laptop</t>
   </si>
 </sst>
 </file>
@@ -408,22 +417,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -432,10 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -755,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F686193E-3E22-4656-9562-EDC82B6A43B5}">
-  <dimension ref="A1:AC22"/>
+  <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH5" sqref="AH5"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -766,9 +775,9 @@
     <col min="1" max="16384" width="5.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -778,11 +787,11 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="11" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
@@ -795,147 +804,143 @@
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="6" t="s">
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="15"/>
+        <v>30</v>
+      </c>
       <c r="E2" s="14" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="H2" s="14"/>
-      <c r="I2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" s="15"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="22"/>
+      <c r="S2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="14"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="17"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="7">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="20"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="16" t="s">
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="F5" s="17"/>
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
@@ -963,33 +968,33 @@
       <c r="O5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="S5" s="23" t="s">
+      <c r="P5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="T5" s="23"/>
-      <c r="W5" s="8"/>
-      <c r="Z5" s="10"/>
-      <c r="AC5" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="V5" s="17"/>
+      <c r="AA5" s="8"/>
+      <c r="AD5" s="10"/>
+      <c r="AF5" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1017,45 +1022,44 @@
       <c r="O6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="8"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="16" t="s">
+      <c r="P6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="8"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="20"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="10"/>
+      <c r="AF6" s="18"/>
+    </row>
+    <row r="7" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="E7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="10"/>
-      <c r="AC6" s="13"/>
-    </row>
-    <row r="7" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="K7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1063,46 +1067,47 @@
         <v>8</v>
       </c>
       <c r="M7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="P7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R7" s="17"/>
-      <c r="S7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="T7" s="1"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="10"/>
-      <c r="AC7" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="T7" s="17"/>
+      <c r="U7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="1"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="10"/>
+      <c r="AF7" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="17"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1133,30 +1138,31 @@
       <c r="P8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="1"/>
-      <c r="U8" s="16" t="s">
+      <c r="Q8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" s="15"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="1"/>
+      <c r="X8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="V8" s="17"/>
-      <c r="W8" s="8"/>
-      <c r="Z8" s="10"/>
-      <c r="AC8" s="13"/>
-    </row>
-    <row r="9" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="17"/>
+      <c r="AD8" s="10"/>
+      <c r="AF8" s="18"/>
+    </row>
+    <row r="9" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1187,42 +1193,43 @@
       <c r="P9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="15" t="s">
+      <c r="Q9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="17"/>
-      <c r="S9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="U9" s="20"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="10"/>
-      <c r="AC9" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="T9" s="17"/>
+      <c r="U9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="19"/>
+      <c r="AB9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="10"/>
+      <c r="AF9" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="I10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1247,33 +1254,34 @@
       <c r="P10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="1"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="10"/>
-      <c r="AB10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC10" s="13"/>
-    </row>
-    <row r="11" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="Q10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="15"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="1"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="19"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="10"/>
+      <c r="AF10" s="18"/>
+      <c r="AI10" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="20"/>
+      <c r="E11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1284,50 +1292,49 @@
         <v>8</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M11" s="13" t="s">
+      <c r="M11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="13"/>
-      <c r="O11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R11" s="1"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="S11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="U11" s="18"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="8"/>
-      <c r="Z11" s="10"/>
-      <c r="AC11" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="20"/>
+      <c r="AD11" s="10"/>
+      <c r="AF11" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1346,102 +1353,108 @@
       <c r="L12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="M12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="15"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="16" t="s">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Y12" s="17"/>
-      <c r="Z12" s="10"/>
-      <c r="AC12" s="13"/>
-    </row>
-    <row r="13" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="10"/>
+      <c r="AF12" s="18"/>
+    </row>
+    <row r="13" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="17"/>
+      <c r="M13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" s="1"/>
+      <c r="S13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V13" s="1"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="10"/>
+      <c r="AF13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="10"/>
-      <c r="AC13" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+    </row>
+    <row r="14" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="Q14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="W14" s="8"/>
-      <c r="Z14" s="10"/>
-      <c r="AC14" s="13"/>
-    </row>
-    <row r="15" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="AA14" s="8"/>
+      <c r="AD14" s="10"/>
+      <c r="AF14" s="18"/>
+    </row>
+    <row r="15" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1462,210 +1475,247 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="16" t="s">
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="Y15" s="17"/>
-      <c r="Z15" s="10"/>
-    </row>
-    <row r="16" spans="1:29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="10"/>
-    </row>
-    <row r="17" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="8"/>
-      <c r="Z17" s="10"/>
-    </row>
-    <row r="18" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="W18" s="8"/>
-      <c r="X18" s="16" t="s">
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="10"/>
+    </row>
+    <row r="16" spans="1:35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="10"/>
+    </row>
+    <row r="17" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="8"/>
+      <c r="AD17" s="10"/>
+    </row>
+    <row r="18" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Y18" s="17"/>
-      <c r="Z18" s="10"/>
-    </row>
-    <row r="19" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="9" t="s">
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="10"/>
+    </row>
+    <row r="19" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="20"/>
+      <c r="AD19" s="10"/>
+    </row>
+    <row r="20" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="5"/>
+    </row>
+    <row r="21" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="AE21" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="10"/>
-    </row>
-    <row r="20" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="5"/>
-    </row>
-    <row r="21" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>49</v>
-      </c>
-      <c r="B21" s="7">
-        <v>49</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA21" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J22" s="7" t="s">
-        <v>41</v>
+      <c r="K22" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="A8:B11"/>
-    <mergeCell ref="U8:V11"/>
-    <mergeCell ref="X18:Y19"/>
-    <mergeCell ref="A16:V17"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="X15:Y16"/>
-    <mergeCell ref="X12:Y13"/>
-    <mergeCell ref="X9:Y10"/>
-    <mergeCell ref="C2:D2"/>
+  <mergeCells count="43">
+    <mergeCell ref="X8:Z11"/>
+    <mergeCell ref="A8:C11"/>
+    <mergeCell ref="W19:X20"/>
+    <mergeCell ref="Y19:Z20"/>
+    <mergeCell ref="A16:Z17"/>
+    <mergeCell ref="M19:N20"/>
+    <mergeCell ref="O19:P20"/>
+    <mergeCell ref="Q19:R20"/>
+    <mergeCell ref="S19:T20"/>
+    <mergeCell ref="U19:V20"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AB3:AC4"/>
+    <mergeCell ref="G3:R4"/>
+    <mergeCell ref="S7:T8"/>
+    <mergeCell ref="S9:T10"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="AB6:AC7"/>
+    <mergeCell ref="U5:V6"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="AC13:AC14"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="X3:Y4"/>
-    <mergeCell ref="E3:P4"/>
-    <mergeCell ref="Q7:R8"/>
-    <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="X6:Y7"/>
-    <mergeCell ref="S5:T6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="AB18:AC19"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="AB15:AC16"/>
+    <mergeCell ref="AB12:AC13"/>
+    <mergeCell ref="AB9:AC10"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:F20"/>
+    <mergeCell ref="G19:H20"/>
+    <mergeCell ref="I19:J20"/>
+    <mergeCell ref="K19:L20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>